<commit_message>
add basic antibio with new data
</commit_message>
<xml_diff>
--- a/static/mock/antibio_data/20.02.2024 AntiBio_дополнено.xlsx
+++ b/static/mock/antibio_data/20.02.2024 AntiBio_дополнено.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexglushko/ProgProjects/ChemML/static/mock/antibio_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexglushko/ProgramProj/ChemML/static/mock/antibio_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122A9D11-0F88-F048-B11D-F48E8B7D4EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E49903-B2CE-734B-90C7-3B50021400AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -8452,9 +8452,6 @@
     <t>Bacteria</t>
   </si>
   <si>
-    <t>Is salt</t>
-  </si>
-  <si>
     <t>Stunting diameter</t>
   </si>
   <si>
@@ -8855,51 +8852,18 @@
     <t>(salt)  d1-1H2O</t>
   </si>
   <si>
-    <t xml:space="preserve">(salt)  d1-2H2O  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(salt)  d1-3H2O  </t>
-  </si>
-  <si>
     <t>(salt) d1-4H2O</t>
   </si>
   <si>
-    <t xml:space="preserve">(salt)  d1-5H2O </t>
-  </si>
-  <si>
     <t>(salt) d1-1NO3</t>
   </si>
   <si>
-    <t xml:space="preserve">(salt) d1-2NO3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(salt) d1-3NO3  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(salt) d1-4NO3    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(salt) d1-5NO3      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(salt) d1-6NO3   </t>
-  </si>
-  <si>
     <t>(salt) d2-1NO3</t>
   </si>
   <si>
-    <t xml:space="preserve">(salt) d2-2NO3  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(salt) d2-3NO3     </t>
-  </si>
-  <si>
     <t>(salt) d3-1H2O</t>
   </si>
   <si>
-    <t xml:space="preserve">(salt) d3-2H2O   </t>
-  </si>
-  <si>
     <t>R1 (Ln-O)</t>
   </si>
   <si>
@@ -9048,6 +9012,42 @@
   </si>
   <si>
     <t>3;7</t>
+  </si>
+  <si>
+    <t>Salt/Solution</t>
+  </si>
+  <si>
+    <t>(salt)  d1-3H2O</t>
+  </si>
+  <si>
+    <t>(salt)  d1-5H2O</t>
+  </si>
+  <si>
+    <t>(salt) d1-2NO3</t>
+  </si>
+  <si>
+    <t>(salt) d1-3NO3</t>
+  </si>
+  <si>
+    <t>(salt) d1-4NO3</t>
+  </si>
+  <si>
+    <t>(salt) d1-5NO3</t>
+  </si>
+  <si>
+    <t>(salt) d1-6NO3</t>
+  </si>
+  <si>
+    <t>(salt) d2-2NO3</t>
+  </si>
+  <si>
+    <t>(salt) d2-3NO3</t>
+  </si>
+  <si>
+    <t>(salt) d3-2H2O</t>
+  </si>
+  <si>
+    <t>(salt)  d1-2H2O</t>
   </si>
 </sst>
 </file>
@@ -10136,11 +10136,11 @@
     <xf numFmtId="49" fontId="0" fillId="24" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -11136,22 +11136,22 @@
     <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="Crystal structure type" dataDxfId="44"/>
     <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="Crystal structure type (literat.)"/>
     <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="(salt)  d1-1H2O" dataDxfId="43"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="(salt)  d1-2H2O  " dataDxfId="42"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="(salt)  d1-3H2O  " dataDxfId="41"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="(salt)  d1-2H2O" dataDxfId="42"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="(salt)  d1-3H2O" dataDxfId="41"/>
     <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="(salt) d1-4H2O" dataDxfId="40"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="(salt)  d1-5H2O " dataDxfId="39"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="(salt)  d1-5H2O" dataDxfId="39"/>
     <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="(salt) d1-1NO3" dataDxfId="38"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="(salt) d1-2NO3 " dataDxfId="37"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="(salt) d1-3NO3  " dataDxfId="36"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="(salt) d1-4NO3    " dataDxfId="35"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="(salt) d1-5NO3      " dataDxfId="34"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="(salt) d1-6NO3   " dataDxfId="33"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="(salt) d1-2NO3" dataDxfId="37"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="(salt) d1-3NO3" dataDxfId="36"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="(salt) d1-4NO3" dataDxfId="35"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="(salt) d1-5NO3" dataDxfId="34"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="(salt) d1-6NO3" dataDxfId="33"/>
     <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="(salt) d1"/>
     <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="(salt) d2-1NO3" dataDxfId="32"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="(salt) d2-2NO3  " dataDxfId="31"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="(salt) d2-3NO3     " dataDxfId="30"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="(salt) d2-2NO3" dataDxfId="31"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="(salt) d2-3NO3" dataDxfId="30"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="(salt) d3-1H2O" dataDxfId="29"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="(salt) d3-2H2O   " dataDxfId="28"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="(salt) d3-2H2O" dataDxfId="28"/>
     <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="Coordination number (solid) Ln-O"/>
     <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="Coordination number (solid) Ln-N"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="x" dataDxfId="27"/>
@@ -11205,7 +11205,7 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="REE" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Bacteria" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Is salt" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Salt/Solution" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Stunting diameter" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -12273,6 +12273,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_CBONDS_CBONDSVARIABLERATETYPE</we:customFunctionIds>
@@ -12431,35 +12434,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="138" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
-      <c r="J1" s="137"/>
-      <c r="K1" s="137"/>
-      <c r="L1" s="137"/>
-      <c r="M1" s="137"/>
-      <c r="N1" s="137"/>
-      <c r="O1" s="137"/>
-      <c r="P1" s="137"/>
-      <c r="Q1" s="137"/>
-      <c r="R1" s="137"/>
-      <c r="S1" s="137"/>
-      <c r="T1" s="137"/>
-      <c r="U1" s="137"/>
-      <c r="V1" s="137"/>
-      <c r="W1" s="137"/>
-      <c r="X1" s="137"/>
-      <c r="Y1" s="137"/>
-      <c r="Z1" s="137"/>
-      <c r="AA1" s="137"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
+      <c r="J1" s="138"/>
+      <c r="K1" s="138"/>
+      <c r="L1" s="138"/>
+      <c r="M1" s="138"/>
+      <c r="N1" s="138"/>
+      <c r="O1" s="138"/>
+      <c r="P1" s="138"/>
+      <c r="Q1" s="138"/>
+      <c r="R1" s="138"/>
+      <c r="S1" s="138"/>
+      <c r="T1" s="138"/>
+      <c r="U1" s="138"/>
+      <c r="V1" s="138"/>
+      <c r="W1" s="138"/>
+      <c r="X1" s="138"/>
+      <c r="Y1" s="138"/>
+      <c r="Z1" s="138"/>
+      <c r="AA1" s="138"/>
     </row>
     <row r="2" spans="1:27" ht="45.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -13186,7 +13189,7 @@
         <v>169</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>170</v>
@@ -13219,13 +13222,13 @@
         <v>82</v>
       </c>
       <c r="R11" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="T11" s="5" t="s">
         <v>408</v>
-      </c>
-      <c r="S11" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="T11" s="5" t="s">
-        <v>409</v>
       </c>
       <c r="U11" s="5" t="s">
         <v>41</v>
@@ -13269,7 +13272,7 @@
         <v>181</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>182</v>
@@ -13302,13 +13305,13 @@
         <v>83</v>
       </c>
       <c r="R12" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="S12" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="T12" s="6" t="s">
         <v>412</v>
-      </c>
-      <c r="S12" s="6" t="s">
-        <v>411</v>
-      </c>
-      <c r="T12" s="6" t="s">
-        <v>413</v>
       </c>
       <c r="U12" s="5" t="s">
         <v>103</v>
@@ -13350,7 +13353,7 @@
         <v>191</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>193</v>
@@ -13431,7 +13434,7 @@
         <v>205</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>206</v>
@@ -13508,7 +13511,7 @@
         <v>33</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>219</v>
@@ -13589,7 +13592,7 @@
         <v>232</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>233</v>
@@ -13867,8 +13870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AR24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13908,88 +13911,88 @@
         <v>262</v>
       </c>
       <c r="B1" s="52" t="s">
+        <v>391</v>
+      </c>
+      <c r="C1" s="97" t="s">
+        <v>395</v>
+      </c>
+      <c r="D1" s="97" t="s">
+        <v>394</v>
+      </c>
+      <c r="E1" s="97" t="s">
+        <v>393</v>
+      </c>
+      <c r="F1" s="97" t="s">
         <v>392</v>
-      </c>
-      <c r="C1" s="97" t="s">
-        <v>396</v>
-      </c>
-      <c r="D1" s="97" t="s">
-        <v>395</v>
-      </c>
-      <c r="E1" s="97" t="s">
-        <v>394</v>
-      </c>
-      <c r="F1" s="97" t="s">
-        <v>393</v>
       </c>
       <c r="G1" s="52" t="s">
         <v>266</v>
       </c>
       <c r="H1" s="52" t="s">
-        <v>475</v>
+        <v>463</v>
       </c>
       <c r="I1" s="90" t="s">
+        <v>420</v>
+      </c>
+      <c r="J1" s="90" t="s">
+        <v>486</v>
+      </c>
+      <c r="K1" s="90" t="s">
+        <v>476</v>
+      </c>
+      <c r="L1" s="90" t="s">
         <v>421</v>
       </c>
-      <c r="J1" s="90" t="s">
+      <c r="M1" s="90" t="s">
+        <v>477</v>
+      </c>
+      <c r="N1" s="94" t="s">
         <v>422</v>
       </c>
-      <c r="K1" s="90" t="s">
+      <c r="O1" s="94" t="s">
+        <v>478</v>
+      </c>
+      <c r="P1" s="94" t="s">
+        <v>479</v>
+      </c>
+      <c r="Q1" s="94" t="s">
+        <v>480</v>
+      </c>
+      <c r="R1" s="94" t="s">
+        <v>481</v>
+      </c>
+      <c r="S1" s="94" t="s">
+        <v>482</v>
+      </c>
+      <c r="T1" s="96" t="s">
+        <v>426</v>
+      </c>
+      <c r="U1" s="95" t="s">
         <v>423</v>
       </c>
-      <c r="L1" s="90" t="s">
+      <c r="V1" s="95" t="s">
+        <v>483</v>
+      </c>
+      <c r="W1" s="95" t="s">
+        <v>484</v>
+      </c>
+      <c r="X1" s="92" t="s">
         <v>424</v>
       </c>
-      <c r="M1" s="90" t="s">
-        <v>425</v>
-      </c>
-      <c r="N1" s="94" t="s">
-        <v>426</v>
-      </c>
-      <c r="O1" s="94" t="s">
-        <v>427</v>
-      </c>
-      <c r="P1" s="94" t="s">
-        <v>428</v>
-      </c>
-      <c r="Q1" s="94" t="s">
-        <v>429</v>
-      </c>
-      <c r="R1" s="94" t="s">
-        <v>430</v>
-      </c>
-      <c r="S1" s="94" t="s">
-        <v>431</v>
-      </c>
-      <c r="T1" s="96" t="s">
-        <v>438</v>
-      </c>
-      <c r="U1" s="95" t="s">
-        <v>432</v>
-      </c>
-      <c r="V1" s="95" t="s">
-        <v>433</v>
-      </c>
-      <c r="W1" s="95" t="s">
-        <v>434</v>
-      </c>
-      <c r="X1" s="92" t="s">
-        <v>435</v>
-      </c>
       <c r="Y1" s="92" t="s">
-        <v>436</v>
+        <v>485</v>
       </c>
       <c r="Z1" s="98" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AA1" s="98" t="s">
-        <v>451</v>
+        <v>439</v>
       </c>
       <c r="AB1" s="52" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="AC1" s="52" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AD1" s="93" t="s">
         <v>263</v>
@@ -14001,34 +14004,34 @@
         <v>265</v>
       </c>
       <c r="AG1" s="93" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AH1" s="91" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="AI1" s="91" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="AJ1" s="101" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
       <c r="AK1" s="91" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="AL1" s="91" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="AM1" s="101" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="AN1" s="131" t="s">
-        <v>472</v>
+        <v>460</v>
       </c>
       <c r="AO1" s="131" t="s">
-        <v>473</v>
+        <v>461</v>
       </c>
       <c r="AP1" s="131" t="s">
-        <v>474</v>
+        <v>462</v>
       </c>
       <c r="AQ1" s="52" t="s">
         <v>268</v>
@@ -15276,8 +15279,8 @@
       <c r="F12" s="81">
         <v>3990</v>
       </c>
-      <c r="G12" s="138" t="s">
-        <v>485</v>
+      <c r="G12" s="137" t="s">
+        <v>473</v>
       </c>
       <c r="H12" s="102">
         <v>3</v>
@@ -15398,8 +15401,8 @@
       <c r="F13" s="82">
         <v>4100</v>
       </c>
-      <c r="G13" s="138" t="s">
-        <v>485</v>
+      <c r="G13" s="137" t="s">
+        <v>473</v>
       </c>
       <c r="H13" s="102">
         <v>3</v>
@@ -15528,8 +15531,8 @@
       <c r="F14" s="81">
         <v>4120</v>
       </c>
-      <c r="G14" s="138" t="s">
-        <v>485</v>
+      <c r="G14" s="137" t="s">
+        <v>473</v>
       </c>
       <c r="H14" s="102">
         <v>3</v>
@@ -15878,8 +15881,8 @@
       <c r="F17" s="81">
         <v>4203</v>
       </c>
-      <c r="G17" s="138" t="s">
-        <v>486</v>
+      <c r="G17" s="137" t="s">
+        <v>474</v>
       </c>
       <c r="H17" s="102">
         <v>3</v>
@@ -16706,7 +16709,7 @@
         <v>316</v>
       </c>
       <c r="N1" s="68" t="s">
-        <v>465</v>
+        <v>453</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -17158,19 +17161,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="129" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="B1" t="s">
-        <v>466</v>
+        <v>454</v>
       </c>
       <c r="C1" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="D1" t="s">
-        <v>467</v>
+        <v>455</v>
       </c>
       <c r="E1" t="s">
-        <v>468</v>
+        <v>456</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -17243,7 +17246,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="128" t="s">
-        <v>469</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -17255,8 +17258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O196"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17281,37 +17284,37 @@
         <v>322</v>
       </c>
       <c r="C1" s="68" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1" s="69" t="s">
         <v>323</v>
       </c>
-      <c r="D1" s="69" t="s">
-        <v>324</v>
-      </c>
       <c r="G1" s="122" t="s">
-        <v>459</v>
+        <v>447</v>
       </c>
       <c r="H1" s="122" t="s">
-        <v>460</v>
+        <v>448</v>
       </c>
       <c r="I1" s="123" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="J1" s="123" t="s">
-        <v>453</v>
+        <v>441</v>
       </c>
       <c r="K1" s="123" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
       <c r="L1" s="123" t="s">
-        <v>455</v>
+        <v>443</v>
       </c>
       <c r="M1" s="123" t="s">
-        <v>456</v>
+        <v>444</v>
       </c>
       <c r="N1" s="123" t="s">
-        <v>457</v>
+        <v>445</v>
       </c>
       <c r="O1" s="123" t="s">
-        <v>458</v>
+        <v>446</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -17328,7 +17331,7 @@
         <v>25</v>
       </c>
       <c r="G2" s="122" t="s">
-        <v>461</v>
+        <v>449</v>
       </c>
       <c r="H2" s="123">
         <v>20</v>
@@ -17410,7 +17413,7 @@
         <v>22</v>
       </c>
       <c r="G4" s="122" t="s">
-        <v>461</v>
+        <v>449</v>
       </c>
       <c r="H4" s="123">
         <v>100</v>
@@ -17451,7 +17454,7 @@
         <v>16</v>
       </c>
       <c r="G5" s="122" t="s">
-        <v>461</v>
+        <v>449</v>
       </c>
       <c r="H5" s="123">
         <v>134</v>
@@ -17492,7 +17495,7 @@
         <v>20</v>
       </c>
       <c r="G6" s="122" t="s">
-        <v>462</v>
+        <v>450</v>
       </c>
       <c r="H6" s="123">
         <v>20</v>
@@ -17533,7 +17536,7 @@
         <v>22</v>
       </c>
       <c r="G7" s="122" t="s">
-        <v>462</v>
+        <v>450</v>
       </c>
       <c r="H7" s="123">
         <v>50</v>
@@ -17574,7 +17577,7 @@
         <v>24</v>
       </c>
       <c r="G8" s="122" t="s">
-        <v>462</v>
+        <v>450</v>
       </c>
       <c r="H8" s="123">
         <v>100</v>
@@ -17615,7 +17618,7 @@
         <v>21</v>
       </c>
       <c r="G9" s="122" t="s">
-        <v>462</v>
+        <v>450</v>
       </c>
       <c r="H9" s="123">
         <v>134</v>
@@ -17656,7 +17659,7 @@
         <v>21</v>
       </c>
       <c r="G10" s="122" t="s">
-        <v>463</v>
+        <v>451</v>
       </c>
       <c r="H10" s="123">
         <v>20</v>
@@ -17697,7 +17700,7 @@
         <v>20</v>
       </c>
       <c r="G11" s="122" t="s">
-        <v>463</v>
+        <v>451</v>
       </c>
       <c r="H11" s="123">
         <v>50</v>
@@ -17738,7 +17741,7 @@
         <v>21</v>
       </c>
       <c r="G12" s="122" t="s">
-        <v>463</v>
+        <v>451</v>
       </c>
       <c r="H12" s="123">
         <v>100</v>
@@ -17779,7 +17782,7 @@
         <v>24</v>
       </c>
       <c r="G13" s="122" t="s">
-        <v>463</v>
+        <v>451</v>
       </c>
       <c r="H13" s="123">
         <v>134</v>
@@ -17820,7 +17823,7 @@
         <v>20</v>
       </c>
       <c r="G14" s="122" t="s">
-        <v>464</v>
+        <v>452</v>
       </c>
       <c r="H14" s="123">
         <v>20</v>
@@ -17861,7 +17864,7 @@
         <v>20</v>
       </c>
       <c r="G15" s="122" t="s">
-        <v>464</v>
+        <v>452</v>
       </c>
       <c r="H15" s="123">
         <v>50</v>
@@ -17902,7 +17905,7 @@
         <v>22</v>
       </c>
       <c r="G16" s="122" t="s">
-        <v>464</v>
+        <v>452</v>
       </c>
       <c r="H16" s="123">
         <v>100</v>
@@ -17943,7 +17946,7 @@
         <v>25</v>
       </c>
       <c r="G17" s="122" t="s">
-        <v>464</v>
+        <v>452</v>
       </c>
       <c r="H17" s="123">
         <v>134</v>
@@ -19893,7 +19896,7 @@
         <v>270</v>
       </c>
       <c r="B155" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C155" s="30">
         <v>1</v>
@@ -19907,7 +19910,7 @@
         <v>272</v>
       </c>
       <c r="B156" s="23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C156" s="29">
         <v>1</v>
@@ -19921,7 +19924,7 @@
         <v>274</v>
       </c>
       <c r="B157" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C157" s="30">
         <v>1</v>
@@ -19935,7 +19938,7 @@
         <v>276</v>
       </c>
       <c r="B158" s="23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C158" s="29">
         <v>1</v>
@@ -19949,7 +19952,7 @@
         <v>278</v>
       </c>
       <c r="B159" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C159" s="30">
         <v>1</v>
@@ -19963,7 +19966,7 @@
         <v>282</v>
       </c>
       <c r="B160" s="23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C160" s="29">
         <v>1</v>
@@ -19977,7 +19980,7 @@
         <v>286</v>
       </c>
       <c r="B161" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C161" s="30">
         <v>1</v>
@@ -19991,7 +19994,7 @@
         <v>288</v>
       </c>
       <c r="B162" s="23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C162" s="29">
         <v>1</v>
@@ -20005,7 +20008,7 @@
         <v>290</v>
       </c>
       <c r="B163" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C163" s="30">
         <v>1</v>
@@ -20019,7 +20022,7 @@
         <v>292</v>
       </c>
       <c r="B164" s="23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C164" s="29">
         <v>1</v>
@@ -20033,7 +20036,7 @@
         <v>293</v>
       </c>
       <c r="B165" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C165" s="30">
         <v>1</v>
@@ -20047,7 +20050,7 @@
         <v>295</v>
       </c>
       <c r="B166" s="23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C166" s="29">
         <v>1</v>
@@ -20061,7 +20064,7 @@
         <v>297</v>
       </c>
       <c r="B167" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C167" s="30">
         <v>1</v>
@@ -20075,7 +20078,7 @@
         <v>299</v>
       </c>
       <c r="B168" s="23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C168" s="29">
         <v>1</v>
@@ -20089,7 +20092,7 @@
         <v>270</v>
       </c>
       <c r="B169" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C169" s="30">
         <v>1</v>
@@ -20103,7 +20106,7 @@
         <v>272</v>
       </c>
       <c r="B170" s="23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C170" s="29">
         <v>1</v>
@@ -20117,7 +20120,7 @@
         <v>274</v>
       </c>
       <c r="B171" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C171" s="30">
         <v>1</v>
@@ -20131,7 +20134,7 @@
         <v>276</v>
       </c>
       <c r="B172" s="23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C172" s="29">
         <v>1</v>
@@ -20145,7 +20148,7 @@
         <v>278</v>
       </c>
       <c r="B173" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C173" s="30">
         <v>1</v>
@@ -20159,7 +20162,7 @@
         <v>282</v>
       </c>
       <c r="B174" s="23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C174" s="29">
         <v>1</v>
@@ -20173,7 +20176,7 @@
         <v>286</v>
       </c>
       <c r="B175" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C175" s="30">
         <v>1</v>
@@ -20187,7 +20190,7 @@
         <v>288</v>
       </c>
       <c r="B176" s="23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C176" s="29">
         <v>1</v>
@@ -20201,7 +20204,7 @@
         <v>290</v>
       </c>
       <c r="B177" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C177" s="30">
         <v>1</v>
@@ -20215,7 +20218,7 @@
         <v>292</v>
       </c>
       <c r="B178" s="23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C178" s="29">
         <v>1</v>
@@ -20229,7 +20232,7 @@
         <v>293</v>
       </c>
       <c r="B179" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C179" s="30">
         <v>1</v>
@@ -20243,7 +20246,7 @@
         <v>295</v>
       </c>
       <c r="B180" s="23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C180" s="29">
         <v>1</v>
@@ -20257,7 +20260,7 @@
         <v>297</v>
       </c>
       <c r="B181" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C181" s="30">
         <v>1</v>
@@ -20271,7 +20274,7 @@
         <v>299</v>
       </c>
       <c r="B182" s="23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C182" s="29">
         <v>1</v>
@@ -20512,7 +20515,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -20525,77 +20528,77 @@
     </row>
     <row r="2" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="105" t="s">
+        <v>327</v>
+      </c>
+      <c r="B2" s="105" t="s">
         <v>328</v>
       </c>
-      <c r="B2" s="105" t="s">
+      <c r="C2" s="105" t="s">
         <v>329</v>
       </c>
-      <c r="C2" s="105" t="s">
+      <c r="D2" s="105" t="s">
         <v>330</v>
       </c>
-      <c r="D2" s="105" t="s">
+      <c r="E2" s="105" t="s">
         <v>331</v>
       </c>
-      <c r="E2" s="105" t="s">
+      <c r="F2" s="105" t="s">
         <v>332</v>
       </c>
-      <c r="F2" s="105" t="s">
+      <c r="G2" s="105" t="s">
         <v>333</v>
       </c>
-      <c r="G2" s="105" t="s">
+      <c r="H2" s="105" t="s">
         <v>334</v>
-      </c>
-      <c r="H2" s="105" t="s">
-        <v>335</v>
       </c>
       <c r="I2" s="32"/>
     </row>
     <row r="3" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="106" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B3" s="106" t="s">
         <v>304</v>
       </c>
       <c r="C3" s="106" t="s">
+        <v>336</v>
+      </c>
+      <c r="D3" s="106" t="s">
         <v>337</v>
       </c>
-      <c r="D3" s="106" t="s">
+      <c r="E3" s="106" t="s">
         <v>338</v>
       </c>
-      <c r="E3" s="106" t="s">
+      <c r="F3" s="106" t="s">
         <v>339</v>
       </c>
-      <c r="F3" s="106" t="s">
+      <c r="G3" s="106" t="s">
         <v>340</v>
       </c>
-      <c r="G3" s="106" t="s">
+      <c r="H3" s="106" t="s">
         <v>341</v>
-      </c>
-      <c r="H3" s="106" t="s">
-        <v>342</v>
       </c>
       <c r="I3" s="104"/>
     </row>
     <row r="4" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="107"/>
       <c r="B4" s="108" t="s">
+        <v>342</v>
+      </c>
+      <c r="C4" s="108" t="s">
         <v>343</v>
       </c>
-      <c r="C4" s="108" t="s">
+      <c r="D4" s="108" t="s">
         <v>344</v>
       </c>
-      <c r="D4" s="108" t="s">
+      <c r="E4" s="108" t="s">
         <v>345</v>
       </c>
-      <c r="E4" s="108" t="s">
+      <c r="F4" s="108" t="s">
         <v>346</v>
       </c>
-      <c r="F4" s="108" t="s">
+      <c r="G4" s="109" t="s">
         <v>347</v>
-      </c>
-      <c r="G4" s="109" t="s">
-        <v>348</v>
       </c>
       <c r="H4" s="110"/>
       <c r="I4" s="104"/>
@@ -20603,18 +20606,18 @@
     <row r="5" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="111"/>
       <c r="B5" s="112" t="s">
+        <v>348</v>
+      </c>
+      <c r="C5" s="112" t="s">
         <v>349</v>
-      </c>
-      <c r="C5" s="112" t="s">
-        <v>350</v>
       </c>
       <c r="D5" s="112"/>
       <c r="E5" s="113"/>
       <c r="F5" s="112" t="s">
+        <v>350</v>
+      </c>
+      <c r="G5" s="114" t="s">
         <v>351</v>
-      </c>
-      <c r="G5" s="114" t="s">
-        <v>352</v>
       </c>
       <c r="H5" s="115"/>
       <c r="I5" s="104"/>
@@ -20622,56 +20625,56 @@
     <row r="6" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="107"/>
       <c r="B6" s="108" t="s">
+        <v>352</v>
+      </c>
+      <c r="C6" s="108" t="s">
         <v>353</v>
       </c>
-      <c r="C6" s="108" t="s">
+      <c r="D6" s="108" t="s">
         <v>354</v>
-      </c>
-      <c r="D6" s="108" t="s">
-        <v>355</v>
       </c>
       <c r="E6" s="116"/>
       <c r="F6" s="116"/>
       <c r="G6" s="109" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H6" s="110" t="s">
-        <v>484</v>
+        <v>472</v>
       </c>
       <c r="I6" s="104"/>
     </row>
     <row r="7" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="107"/>
       <c r="B7" s="108" t="s">
-        <v>475</v>
+        <v>463</v>
       </c>
       <c r="C7" s="108"/>
       <c r="D7" s="108"/>
       <c r="E7" s="116"/>
       <c r="F7" s="116"/>
       <c r="G7" s="109" t="s">
-        <v>476</v>
+        <v>464</v>
       </c>
       <c r="H7" s="110" t="s">
-        <v>483</v>
+        <v>471</v>
       </c>
       <c r="I7" s="104"/>
     </row>
     <row r="8" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="111"/>
       <c r="B8" s="112" t="s">
+        <v>356</v>
+      </c>
+      <c r="C8" s="112" t="s">
         <v>357</v>
       </c>
-      <c r="C8" s="112" t="s">
+      <c r="D8" s="112" t="s">
         <v>358</v>
-      </c>
-      <c r="D8" s="112" t="s">
-        <v>359</v>
       </c>
       <c r="E8" s="113"/>
       <c r="F8" s="113"/>
       <c r="G8" s="114" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H8" s="115"/>
       <c r="I8" s="104"/>
@@ -20679,18 +20682,18 @@
     <row r="9" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="107"/>
       <c r="B9" s="108" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="C9" s="108" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D9" s="108" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E9" s="116"/>
       <c r="F9" s="116"/>
       <c r="G9" s="109" t="s">
-        <v>448</v>
+        <v>436</v>
       </c>
       <c r="H9" s="110"/>
       <c r="I9" s="104"/>
@@ -20698,16 +20701,16 @@
     <row r="10" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="107"/>
       <c r="B10" s="108" t="s">
-        <v>447</v>
+        <v>435</v>
       </c>
       <c r="C10" s="108"/>
       <c r="D10" s="108" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E10" s="116"/>
       <c r="F10" s="116"/>
       <c r="G10" s="109" t="s">
-        <v>449</v>
+        <v>437</v>
       </c>
       <c r="H10" s="110"/>
       <c r="I10" s="104"/>
@@ -20715,16 +20718,16 @@
     <row r="11" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="107"/>
       <c r="B11" s="108" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="C11" s="108"/>
       <c r="D11" s="108" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E11" s="116"/>
       <c r="F11" s="116"/>
       <c r="G11" s="109" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="H11" s="110"/>
       <c r="I11" s="104"/>
@@ -20732,10 +20735,10 @@
     <row r="12" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="111"/>
       <c r="B12" s="112" t="s">
+        <v>361</v>
+      </c>
+      <c r="C12" s="112" t="s">
         <v>362</v>
-      </c>
-      <c r="C12" s="112" t="s">
-        <v>363</v>
       </c>
       <c r="D12" s="112" t="s">
         <v>267</v>
@@ -20743,7 +20746,7 @@
       <c r="E12" s="113"/>
       <c r="F12" s="113"/>
       <c r="G12" s="114" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H12" s="115"/>
       <c r="I12" s="104"/>
@@ -20751,20 +20754,20 @@
     <row r="13" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="107"/>
       <c r="B13" s="108" t="s">
+        <v>364</v>
+      </c>
+      <c r="C13" s="108" t="s">
+        <v>468</v>
+      </c>
+      <c r="D13" s="108" t="s">
         <v>365</v>
-      </c>
-      <c r="C13" s="108" t="s">
-        <v>480</v>
-      </c>
-      <c r="D13" s="108" t="s">
-        <v>366</v>
       </c>
       <c r="E13" s="116"/>
       <c r="F13" s="116" t="s">
-        <v>482</v>
+        <v>470</v>
       </c>
       <c r="G13" s="109" t="s">
-        <v>481</v>
+        <v>469</v>
       </c>
       <c r="H13" s="110"/>
       <c r="I13" s="104"/>
@@ -20772,16 +20775,16 @@
     <row r="14" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="107"/>
       <c r="B14" s="108" t="s">
-        <v>479</v>
+        <v>467</v>
       </c>
       <c r="C14" s="108"/>
       <c r="D14" s="108" t="s">
-        <v>477</v>
+        <v>465</v>
       </c>
       <c r="E14" s="116"/>
       <c r="F14" s="116"/>
       <c r="G14" s="109" t="s">
-        <v>478</v>
+        <v>466</v>
       </c>
       <c r="H14" s="110"/>
       <c r="I14" s="104"/>
@@ -20789,18 +20792,18 @@
     <row r="15" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="111"/>
       <c r="B15" s="112" t="s">
+        <v>366</v>
+      </c>
+      <c r="C15" s="112" t="s">
         <v>367</v>
       </c>
-      <c r="C15" s="112" t="s">
+      <c r="D15" s="112" t="s">
         <v>368</v>
-      </c>
-      <c r="D15" s="112" t="s">
-        <v>369</v>
       </c>
       <c r="E15" s="113"/>
       <c r="F15" s="113"/>
       <c r="G15" s="114" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H15" s="115"/>
       <c r="I15" s="104"/>
@@ -20808,18 +20811,18 @@
     <row r="16" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="107"/>
       <c r="B16" s="108" t="s">
+        <v>370</v>
+      </c>
+      <c r="C16" s="108" t="s">
         <v>371</v>
       </c>
-      <c r="C16" s="108" t="s">
+      <c r="D16" s="108" t="s">
         <v>372</v>
-      </c>
-      <c r="D16" s="108" t="s">
-        <v>373</v>
       </c>
       <c r="E16" s="116"/>
       <c r="F16" s="116"/>
       <c r="G16" s="109" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H16" s="110"/>
       <c r="I16" s="104"/>
@@ -20827,16 +20830,16 @@
     <row r="17" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="117"/>
       <c r="B17" s="117" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C17" s="117"/>
       <c r="D17" s="117"/>
       <c r="E17" s="117"/>
       <c r="F17" s="117" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G17" s="117" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H17" s="117"/>
       <c r="I17" s="104"/>
@@ -20844,122 +20847,122 @@
     <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="118"/>
       <c r="B18" s="119" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
       <c r="C18" s="118"/>
       <c r="D18" s="118"/>
       <c r="E18" s="118" t="s">
+        <v>345</v>
+      </c>
+      <c r="F18" s="118" t="s">
         <v>346</v>
       </c>
-      <c r="F18" s="118" t="s">
-        <v>347</v>
-      </c>
       <c r="G18" s="119" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H18" s="118"/>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="118"/>
       <c r="B19" s="119" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C19" s="118"/>
       <c r="D19" s="118"/>
       <c r="E19" s="118" t="s">
+        <v>345</v>
+      </c>
+      <c r="F19" s="119" t="s">
         <v>346</v>
       </c>
-      <c r="F19" s="119" t="s">
-        <v>347</v>
-      </c>
       <c r="G19" s="118" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H19" s="118"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="118"/>
       <c r="B20" s="119" t="s">
-        <v>445</v>
+        <v>433</v>
       </c>
       <c r="C20" s="118"/>
       <c r="D20" s="118"/>
       <c r="E20" s="118" t="s">
+        <v>345</v>
+      </c>
+      <c r="F20" s="119" t="s">
         <v>346</v>
       </c>
-      <c r="F20" s="119" t="s">
-        <v>347</v>
-      </c>
       <c r="G20" s="118" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
       <c r="H20" s="118"/>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="118"/>
       <c r="B21" s="119" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="C21" s="118"/>
       <c r="D21" s="118"/>
       <c r="E21" s="119" t="s">
+        <v>345</v>
+      </c>
+      <c r="F21" s="118" t="s">
         <v>346</v>
       </c>
-      <c r="F21" s="118" t="s">
-        <v>347</v>
-      </c>
       <c r="G21" s="119" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H21" s="118"/>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="118"/>
       <c r="B22" s="119" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C22" s="118"/>
       <c r="D22" s="118"/>
       <c r="E22" s="119" t="s">
+        <v>345</v>
+      </c>
+      <c r="F22" s="119" t="s">
         <v>346</v>
       </c>
-      <c r="F22" s="119" t="s">
-        <v>347</v>
-      </c>
       <c r="G22" s="119" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H22" s="118"/>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="118"/>
       <c r="B23" s="120" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C23" s="118" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D23" s="121"/>
       <c r="E23" s="118"/>
       <c r="F23" s="118"/>
       <c r="G23" s="121" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H23" s="118"/>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="118"/>
       <c r="B24" s="120" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C24" s="118" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D24" s="118"/>
       <c r="E24" s="118"/>
       <c r="F24" s="118"/>
       <c r="G24" s="121" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H24" s="118"/>
     </row>
@@ -20990,7 +20993,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
@@ -21001,22 +21004,22 @@
     </row>
     <row r="2" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="35" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B2" s="36" t="s">
         <v>304</v>
       </c>
       <c r="C2" s="36" t="s">
+        <v>375</v>
+      </c>
+      <c r="D2" s="36" t="s">
         <v>376</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="E2" s="36" t="s">
         <v>377</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="F2" s="37" t="s">
         <v>378</v>
-      </c>
-      <c r="F2" s="37" t="s">
-        <v>379</v>
       </c>
       <c r="G2" s="38"/>
     </row>
@@ -21025,16 +21028,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="40" t="s">
+        <v>379</v>
+      </c>
+      <c r="C3" s="40" t="s">
         <v>380</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="D3" s="40" t="s">
+        <v>380</v>
+      </c>
+      <c r="E3" s="40" t="s">
         <v>381</v>
-      </c>
-      <c r="D3" s="40" t="s">
-        <v>381</v>
-      </c>
-      <c r="E3" s="40" t="s">
-        <v>382</v>
       </c>
       <c r="F3" s="41">
         <v>1496</v>
@@ -21046,16 +21049,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="43" t="s">
+        <v>382</v>
+      </c>
+      <c r="C4" s="43" t="s">
         <v>383</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="D4" s="43" t="s">
+        <v>383</v>
+      </c>
+      <c r="E4" s="43" t="s">
         <v>384</v>
-      </c>
-      <c r="D4" s="43" t="s">
-        <v>384</v>
-      </c>
-      <c r="E4" s="43" t="s">
-        <v>385</v>
       </c>
       <c r="F4" s="44">
         <v>585</v>
@@ -21067,16 +21070,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="C5" s="40" t="s">
         <v>386</v>
       </c>
-      <c r="C5" s="40" t="s">
-        <v>387</v>
-      </c>
       <c r="D5" s="40" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F5" s="41">
         <v>59201</v>
@@ -21088,16 +21091,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="43" t="s">
+        <v>387</v>
+      </c>
+      <c r="C6" s="43" t="s">
         <v>388</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="D6" s="43" t="s">
         <v>389</v>
       </c>
-      <c r="D6" s="43" t="s">
-        <v>390</v>
-      </c>
       <c r="E6" s="43" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F6" s="44">
         <v>622</v>
@@ -21109,7 +21112,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C7" s="40" t="s">
         <v>23</v>
@@ -21118,7 +21121,7 @@
         <v>23</v>
       </c>
       <c r="E7" s="40" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F7" s="41">
         <v>470</v>

</xml_diff>